<commit_message>
feat(import): dynamic preview table and mapping dropdown includes all DB columns and new fields
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krishna/requirement-prioritizer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8EF53F4F-17D9-8A4E-8D37-7052B8810AAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A35C991E-2BBF-794B-8C04-0A192710DCE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4440" yWindow="2260" windowWidth="20520" windowHeight="14020" xr2:uid="{AF30DAEB-28D2-DD46-9931-5F1C40808B43}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Key</t>
   </si>
@@ -63,6 +63,15 @@
   </si>
   <si>
     <t>Low</t>
+  </si>
+  <si>
+    <t>Product Owner</t>
+  </si>
+  <si>
+    <t>PO1</t>
+  </si>
+  <si>
+    <t>PO2</t>
   </si>
 </sst>
 </file>
@@ -444,15 +453,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FE0A45F-1BE2-FB40-AABA-48457DBB0999}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -462,8 +474,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -473,8 +488,11 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -483,6 +501,9 @@
       </c>
       <c r="C3" t="s">
         <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>